<commit_message>
Start on Foundational Services & APIC & LDAP
</commit_message>
<xml_diff>
--- a/doc/SomeData.xlsx
+++ b/doc/SomeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CurrentProjects\CP4I\Installation\cp4i-install\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14B5B3E-89AA-43D0-B3EB-A67451B78324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBF2402-FF07-4DB1-BD37-E273ABD009FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1164" yWindow="3228" windowWidth="18438" windowHeight="9654" xr2:uid="{0319FF5B-C6C8-4DE2-B9EA-9514F46FE056}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0319FF5B-C6C8-4DE2-B9EA-9514F46FE056}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,12 +169,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609BF403-B9AA-45B0-8B24-6344D6FA7A9F}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -515,10 +514,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>2400</v>
       </c>
       <c r="C2">
@@ -696,7 +695,7 @@
         <v>6.2500000000000001E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -708,7 +707,7 @@
         <v>6.7129629629629625E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -720,7 +719,7 @@
         <v>7.407407407407407E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -732,7 +731,7 @@
         <v>1.9675925925925924E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C20">
         <f>SUM(B14:B19)</f>
         <v>741</v>
@@ -742,7 +741,7 @@
         <v>8.5763888888888886E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -757,7 +756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -769,7 +768,7 @@
         <v>2.0601851851851853E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -781,7 +780,7 @@
         <v>4.5023148148148149E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -793,7 +792,7 @@
         <v>2.0173611111111111E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -805,7 +804,7 @@
         <v>2.5231481481481481E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -816,26 +815,36 @@
         <f t="shared" si="1"/>
         <v>4.9189814814814816E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="H26">
+        <v>7669</v>
+      </c>
+      <c r="I26">
+        <f>7669/3600</f>
+        <v>2.1302777777777777</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C27">
         <f>SUM(B21:B26)</f>
         <v>5448</v>
       </c>
-      <c r="D27">
+      <c r="E27" s="2">
+        <f>C27/86400</f>
+        <v>6.3055555555555559E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
         <f>SUM(C2:C27)</f>
         <v>9194</v>
       </c>
-      <c r="E27" s="2">
-        <f>D27/86400</f>
+      <c r="E28" s="2">
+        <f>C28/86400</f>
         <v>0.10641203703703704</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E28" xr:uid="{609BF403-B9AA-45B0-8B24-6344D6FA7A9F}"/>

</xml_diff>

<commit_message>
Broken wait for state
</commit_message>
<xml_diff>
--- a/doc/SomeData.xlsx
+++ b/doc/SomeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBF2402-FF07-4DB1-BD37-E273ABD009FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD0BEC7-88E2-4138-84C9-4E65C482B14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0319FF5B-C6C8-4DE2-B9EA-9514F46FE056}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{0319FF5B-C6C8-4DE2-B9EA-9514F46FE056}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>To have ingress available</t>
   </si>
@@ -123,6 +123,75 @@
   </si>
   <si>
     <t>Cluster creation</t>
+  </si>
+  <si>
+    <t>Checking Ingress availability</t>
+  </si>
+  <si>
+    <t>Adding case ibm-licensing</t>
+  </si>
+  <si>
+    <t>Creation of openshift-cert-manager-operator operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-licensing-operator-app operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-common-service-operator operator</t>
+  </si>
+  <si>
+    <t>Creation of commonservice instance</t>
+  </si>
+  <si>
+    <t>Creation of APIConnectCluster instance</t>
+  </si>
+  <si>
+    <t>2023.4 2 january 2024</t>
+  </si>
+  <si>
+    <t>Adding case ibm-eventendpointmanagement</t>
+  </si>
+  <si>
+    <t>Adding case ibm-eventprocessing</t>
+  </si>
+  <si>
+    <t>Adding case ibm-eventautomation-flink</t>
+  </si>
+  <si>
+    <t>Creation of datapower-operator operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-eventendpointmanagement operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-eventautomation-flink.v1.1.1 operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-eventprocessing.v1.1.1 operator</t>
+  </si>
+  <si>
+    <t>Creation of Dashboard instance</t>
+  </si>
+  <si>
+    <t>Creation of DesignerAuthoring instance</t>
+  </si>
+  <si>
+    <t>Creation of EventStreams instance</t>
+  </si>
+  <si>
+    <t>Creation of EventEndpointManagement instance</t>
+  </si>
+  <si>
+    <t>Creation of EventGateway instance</t>
+  </si>
+  <si>
+    <t>Creation of PersistentVolumeClaim instance</t>
+  </si>
+  <si>
+    <t>Creation of FlinkDeployment instance</t>
+  </si>
+  <si>
+    <t>Creation of EventProcessing instance</t>
   </si>
 </sst>
 </file>
@@ -132,7 +201,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +213,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,11 +246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -338,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -480,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,18 +566,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609BF403-B9AA-45B0-8B24-6344D6FA7A9F}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="48.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="4.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -846,6 +924,568 @@
         <v>0.10641203703703704</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <v>56</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" ref="E34:E44" si="2">B34/86400</f>
+        <v>6.4814814814814813E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="2"/>
+        <v>8.1018518518518516E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="2"/>
+        <v>4.6296296296296294E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0416666666666667E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39">
+        <v>55</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3657407407407413E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40">
+        <v>51</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="2"/>
+        <v>5.9027777777777778E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>41</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="2"/>
+        <v>4.7453703703703704E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>51</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="2"/>
+        <v>5.9027777777777778E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>55</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3657407407407413E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45">
+        <v>1380</v>
+      </c>
+      <c r="E45" s="3">
+        <f>B45/86400</f>
+        <v>1.5972222222222221E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="1">
+        <f>SUM(B34:B45)</f>
+        <v>1713</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2">
+        <f>B46/86400</f>
+        <v>1.982638888888889E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>20240116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>1005</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" ref="E51:E83" si="3">B51/86400</f>
+        <v>1.1631944444444445E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="3"/>
+        <v>4.6296296296296294E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62">
+        <v>98</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1342592592592593E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63">
+        <v>71</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="3"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64">
+        <v>47</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4398148148148144E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65">
+        <v>47</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4398148148148144E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>49</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="3"/>
+        <v>5.6712962962962967E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67">
+        <v>46</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="3"/>
+        <v>5.3240740740740744E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68">
+        <v>52</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="3"/>
+        <v>6.018518518518519E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69">
+        <v>95</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0995370370370371E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70">
+        <v>65</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="3"/>
+        <v>7.5231481481481482E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="3"/>
+        <v>7.8703703703703705E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <v>188</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1759259259259258E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73">
+        <v>56</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="3"/>
+        <v>6.4814814814814813E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74">
+        <v>119</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3773148148148147E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75">
+        <v>5925</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" si="3"/>
+        <v>6.8576388888888895E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76">
+        <v>1407</v>
+      </c>
+      <c r="E76" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6284722222222221E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B77">
+        <v>652</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="3"/>
+        <v>7.5462962962962966E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0416666666666667E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="3"/>
+        <v>8.1018518518518516E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80">
+        <v>70</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" si="3"/>
+        <v>8.1018518518518516E-4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81">
+        <v>139</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6087962962962963E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82">
+        <v>264</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="3"/>
+        <v>3.0555555555555557E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B83" s="1">
+        <f>SUM(B51:B82)</f>
+        <v>10500</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12152777777777778</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E28" xr:uid="{609BF403-B9AA-45B0-8B24-6344D6FA7A9F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SB]20240506 nouvelle branche sb
</commit_message>
<xml_diff>
--- a/doc/SomeData.xlsx
+++ b/doc/SomeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBF2402-FF07-4DB1-BD37-E273ABD009FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD0BEC7-88E2-4138-84C9-4E65C482B14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0319FF5B-C6C8-4DE2-B9EA-9514F46FE056}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{0319FF5B-C6C8-4DE2-B9EA-9514F46FE056}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>To have ingress available</t>
   </si>
@@ -123,6 +123,75 @@
   </si>
   <si>
     <t>Cluster creation</t>
+  </si>
+  <si>
+    <t>Checking Ingress availability</t>
+  </si>
+  <si>
+    <t>Adding case ibm-licensing</t>
+  </si>
+  <si>
+    <t>Creation of openshift-cert-manager-operator operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-licensing-operator-app operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-common-service-operator operator</t>
+  </si>
+  <si>
+    <t>Creation of commonservice instance</t>
+  </si>
+  <si>
+    <t>Creation of APIConnectCluster instance</t>
+  </si>
+  <si>
+    <t>2023.4 2 january 2024</t>
+  </si>
+  <si>
+    <t>Adding case ibm-eventendpointmanagement</t>
+  </si>
+  <si>
+    <t>Adding case ibm-eventprocessing</t>
+  </si>
+  <si>
+    <t>Adding case ibm-eventautomation-flink</t>
+  </si>
+  <si>
+    <t>Creation of datapower-operator operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-eventendpointmanagement operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-eventautomation-flink.v1.1.1 operator</t>
+  </si>
+  <si>
+    <t>Creation of ibm-eventprocessing.v1.1.1 operator</t>
+  </si>
+  <si>
+    <t>Creation of Dashboard instance</t>
+  </si>
+  <si>
+    <t>Creation of DesignerAuthoring instance</t>
+  </si>
+  <si>
+    <t>Creation of EventStreams instance</t>
+  </si>
+  <si>
+    <t>Creation of EventEndpointManagement instance</t>
+  </si>
+  <si>
+    <t>Creation of EventGateway instance</t>
+  </si>
+  <si>
+    <t>Creation of PersistentVolumeClaim instance</t>
+  </si>
+  <si>
+    <t>Creation of FlinkDeployment instance</t>
+  </si>
+  <si>
+    <t>Creation of EventProcessing instance</t>
   </si>
 </sst>
 </file>
@@ -132,7 +201,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +213,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,11 +246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -338,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -480,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,18 +566,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609BF403-B9AA-45B0-8B24-6344D6FA7A9F}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="48.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="4.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -846,6 +924,568 @@
         <v>0.10641203703703704</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <v>56</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" ref="E34:E44" si="2">B34/86400</f>
+        <v>6.4814814814814813E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="2"/>
+        <v>8.1018518518518516E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="2"/>
+        <v>4.6296296296296294E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0416666666666667E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39">
+        <v>55</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3657407407407413E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40">
+        <v>51</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="2"/>
+        <v>5.9027777777777778E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>41</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="2"/>
+        <v>4.7453703703703704E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>51</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="2"/>
+        <v>5.9027777777777778E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>55</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3657407407407413E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45">
+        <v>1380</v>
+      </c>
+      <c r="E45" s="3">
+        <f>B45/86400</f>
+        <v>1.5972222222222221E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="1">
+        <f>SUM(B34:B45)</f>
+        <v>1713</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2">
+        <f>B46/86400</f>
+        <v>1.982638888888889E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>20240116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>1005</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" ref="E51:E83" si="3">B51/86400</f>
+        <v>1.1631944444444445E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="3"/>
+        <v>4.6296296296296294E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62">
+        <v>98</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1342592592592593E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63">
+        <v>71</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="3"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64">
+        <v>47</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4398148148148144E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65">
+        <v>47</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4398148148148144E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>49</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="3"/>
+        <v>5.6712962962962967E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67">
+        <v>46</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="3"/>
+        <v>5.3240740740740744E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68">
+        <v>52</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="3"/>
+        <v>6.018518518518519E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69">
+        <v>95</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0995370370370371E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70">
+        <v>65</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="3"/>
+        <v>7.5231481481481482E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="3"/>
+        <v>7.8703703703703705E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <v>188</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1759259259259258E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73">
+        <v>56</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="3"/>
+        <v>6.4814814814814813E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74">
+        <v>119</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3773148148148147E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75">
+        <v>5925</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" si="3"/>
+        <v>6.8576388888888895E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76">
+        <v>1407</v>
+      </c>
+      <c r="E76" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6284722222222221E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B77">
+        <v>652</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="3"/>
+        <v>7.5462962962962966E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0416666666666667E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="3"/>
+        <v>8.1018518518518516E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80">
+        <v>70</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" si="3"/>
+        <v>8.1018518518518516E-4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81">
+        <v>139</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6087962962962963E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82">
+        <v>264</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="3"/>
+        <v>3.0555555555555557E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B83" s="1">
+        <f>SUM(B51:B82)</f>
+        <v>10500</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12152777777777778</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E28" xr:uid="{609BF403-B9AA-45B0-8B24-6344D6FA7A9F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>